<commit_message>
added final names to table
</commit_message>
<xml_diff>
--- a/data/old2newfamilynames.xlsx
+++ b/data/old2newfamilynames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idamei/phd/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4578F7B-A82B-4141-A9AC-74723BEC40ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC1F0B-E416-124C-92D3-4F6329BDD270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{639F621F-E074-864A-87C7-16ACDEDF2CCC}"/>
+    <workbookView xWindow="16000" yWindow="-22700" windowWidth="30240" windowHeight="18880" xr2:uid="{639F621F-E074-864A-87C7-16ACDEDF2CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>old_name</t>
   </si>
@@ -144,16 +144,76 @@
   </si>
   <si>
     <t>X615</t>
+  </si>
+  <si>
+    <t>new_new_name</t>
+  </si>
+  <si>
+    <t>GT119</t>
+  </si>
+  <si>
+    <t>GT120</t>
+  </si>
+  <si>
+    <t>GT121</t>
+  </si>
+  <si>
+    <t>GT122</t>
+  </si>
+  <si>
+    <t>GT123</t>
+  </si>
+  <si>
+    <t>GT124</t>
+  </si>
+  <si>
+    <t>GT125</t>
+  </si>
+  <si>
+    <t>GT126</t>
+  </si>
+  <si>
+    <t>GT127</t>
+  </si>
+  <si>
+    <t>GT128</t>
+  </si>
+  <si>
+    <t>GT129</t>
+  </si>
+  <si>
+    <t>GT130</t>
+  </si>
+  <si>
+    <t>GT131</t>
+  </si>
+  <si>
+    <t>GT132</t>
+  </si>
+  <si>
+    <t>GT133</t>
+  </si>
+  <si>
+    <t>GT134</t>
+  </si>
+  <si>
+    <t>GT135</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,9 +259,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -239,7 +299,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -345,7 +405,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -495,159 +555,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF518533-1F6E-F249-AFCB-313C23383B03}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>